<commit_message>
added a list of recipients
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rubin\PycharmProjects\Charcoal\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rubin\PycharmProjects\Charcoal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D87AFC5-69FC-4958-AD98-7431B00E6AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9741122E-025C-4E07-95FF-E340B09CE947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0DD7FB95-636C-47AB-B62C-6E220D87849D}"/>
   </bookViews>
@@ -36,33 +36,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t>Уголь березовый 10 литров  (2,2кг)</t>
-  </si>
-  <si>
-    <t>Уголь березовый 20 литров  (4,5кг)</t>
-  </si>
-  <si>
-    <t>Уголь березовый 50л  (9кг)</t>
-  </si>
-  <si>
-    <t>Древесно-угольный микс 7л  (3кг)</t>
-  </si>
-  <si>
-    <t>Уголь древесный 10 л  ( 0,9 – 1 кг)</t>
-  </si>
-  <si>
-    <t>Уголь древесный 20 л   ( 1,8 – 2 кг)</t>
-  </si>
-  <si>
     <t>Уголь древесно-брикетный (евроуголь) 10 кг</t>
   </si>
   <si>
     <t>Уголь брикетный 10 кг в коробке</t>
   </si>
   <si>
-    <t>Уголь березовый 10 литров  (2 кг) (эконом)</t>
-  </si>
-  <si>
     <t>Наличный расчет</t>
   </si>
   <si>
@@ -73,6 +52,27 @@
   </si>
   <si>
     <t>Наименование</t>
+  </si>
+  <si>
+    <t>Уголь древесный 10 л</t>
+  </si>
+  <si>
+    <t>Уголь древесный 20 л</t>
+  </si>
+  <si>
+    <t>Уголь березовый 10 литров</t>
+  </si>
+  <si>
+    <t>Уголь березовый 20 литров</t>
+  </si>
+  <si>
+    <t>Уголь березовый 10 литров (эконом)</t>
+  </si>
+  <si>
+    <t>Древесно-угольный микс 3кг</t>
+  </si>
+  <si>
+    <t>Уголь березовый 50л (10кг)</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -448,142 +448,142 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C2" s="1">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="D2" s="1">
-        <v>156</v>
+        <v>175.2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="C3" s="1">
-        <v>260</v>
+        <v>286</v>
       </c>
       <c r="D3" s="1">
-        <v>312</v>
+        <v>343.2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="C4" s="1">
-        <v>480</v>
+        <v>550</v>
       </c>
       <c r="D4" s="1">
-        <v>576</v>
+        <v>660</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C5" s="1">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="D5" s="1">
-        <v>132</v>
+        <v>160.80000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="C6" s="1">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="D6" s="1">
-        <v>240</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1">
-        <v>50</v>
+        <v>60.5</v>
       </c>
       <c r="D7" s="1">
-        <v>60</v>
+        <v>72.599999999999994</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="C8" s="1">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="D8" s="1">
-        <v>126</v>
+        <v>145.19999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B9" s="1">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="C9" s="1">
-        <v>480</v>
+        <v>550</v>
       </c>
       <c r="D9" s="1">
-        <v>576</v>
+        <v>660</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1">
         <v>450</v>
       </c>
       <c r="C10" s="1">
-        <v>480</v>
+        <v>495</v>
       </c>
       <c r="D10" s="1">
-        <v>576</v>
+        <v>594</v>
       </c>
     </row>
   </sheetData>

</xml_diff>